<commit_message>
UI with Cable Sizing
</commit_message>
<xml_diff>
--- a/Messenger Cable Sizes.xlsx
+++ b/Messenger Cable Sizes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_2d1a\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roneill\Documents\CRO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{173153F4-264B-43FF-AA34-D5EC513F4D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1EC507-5407-4B8B-8F68-0F38DAB1EF81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14745" yWindow="330" windowWidth="13440" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Size</t>
   </si>
@@ -41,12 +42,6 @@
     <t>Diameter</t>
   </si>
   <si>
-    <t>Radius</t>
-  </si>
-  <si>
-    <t>LB Per Foot</t>
-  </si>
-  <si>
     <t>Cross Sect. Area</t>
   </si>
   <si>
@@ -63,13 +58,46 @@
   </si>
   <si>
     <t>7C#10</t>
+  </si>
+  <si>
+    <t>2C#4</t>
+  </si>
+  <si>
+    <t>2C#6</t>
+  </si>
+  <si>
+    <t>2C#9</t>
+  </si>
+  <si>
+    <t>2C#14</t>
+  </si>
+  <si>
+    <t>3C#4</t>
+  </si>
+  <si>
+    <t>3C#6</t>
+  </si>
+  <si>
+    <t>10C#14</t>
+  </si>
+  <si>
+    <t>12C#14</t>
+  </si>
+  <si>
+    <t>14C#14</t>
+  </si>
+  <si>
+    <t>25C#14</t>
+  </si>
+  <si>
+    <t>Lb Per Foot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,8 +574,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -903,100 +932,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0.9</v>
+      </c>
+      <c r="C2">
+        <v>0.86</v>
+      </c>
+      <c r="D2">
+        <f>ROUND(PI() * ((B2/2)^2), 2)</f>
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>1.3</v>
+      </c>
+      <c r="C3">
+        <v>0.96</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="0">ROUND(PI() * ((B3/2)^2), 2)</f>
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>1.175</v>
+      </c>
+      <c r="C4">
+        <v>0.73499999999999999</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="C2">
-        <v>0.47299999999999998</v>
-      </c>
-      <c r="D2">
-        <v>0.874</v>
-      </c>
-      <c r="E2">
-        <v>0.70099999999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B5">
+        <v>0.99</v>
+      </c>
+      <c r="C5">
+        <v>0.495</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
-      </c>
-      <c r="B3">
-        <v>1.51</v>
-      </c>
-      <c r="C3">
-        <v>0.755</v>
-      </c>
-      <c r="D3">
-        <v>1.284</v>
-      </c>
-      <c r="E3">
-        <v>1.7909999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>0.99</v>
-      </c>
-      <c r="C4">
-        <v>0.495</v>
-      </c>
-      <c r="D4">
-        <v>0.495</v>
-      </c>
-      <c r="E4">
-        <v>0.76900000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5">
-        <v>1.4850000000000001</v>
-      </c>
-      <c r="C5">
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="D5">
-        <v>0.74299999999999999</v>
-      </c>
-      <c r="E5">
-        <v>1.734</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>9</v>
       </c>
       <c r="B6">
         <v>1.4850000000000001</v>
@@ -1005,10 +1031,134 @@
         <v>0.74299999999999999</v>
       </c>
       <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="C7">
         <v>0.74299999999999999</v>
       </c>
-      <c r="E6">
-        <v>1.734</v>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>1.232</v>
+      </c>
+      <c r="C8">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="D8">
+        <f>ROUND(PI() * ((B8/2)^2), 2)</f>
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>1.27</v>
+      </c>
+      <c r="C9">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="D9">
+        <f>ROUND(PI() * ((B9/2)^2), 2)</f>
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>1.3320000000000001</v>
+      </c>
+      <c r="C10">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="D10">
+        <f>ROUND(PI() * ((B10/2)^2), 2)</f>
+        <v>1.39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1.5069999999999999</v>
+      </c>
+      <c r="C11">
+        <v>1.284</v>
+      </c>
+      <c r="D11">
+        <f>ROUND(PI() * ((B11/2)^2), 2)</f>
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>1.24</v>
+      </c>
+      <c r="C12">
+        <v>0.88</v>
+      </c>
+      <c r="D12">
+        <f>ROUND(PI() * ((B12/2)^2), 2)</f>
+        <v>1.21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92E7ED7-8DAC-4334-B6A0-FB5C45401068}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>